<commit_message>
start making q excel data
</commit_message>
<xml_diff>
--- a/scapp/modules/temp.xlsx
+++ b/scapp/modules/temp.xlsx
@@ -7,14 +7,14 @@
   </bookViews>
   <sheets>
     <sheet name="表紙" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="基本" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="総合健康リスク" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -27,6 +27,12 @@
       <name val="Aptos Narrow"/>
       <sz val="18"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <sz val="14"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -36,7 +42,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -44,13 +50,76 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="7" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="8" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="9" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -65,10 +134,10 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2160000" cy="1440000"/>
+    <xdr:ext cx="6480000" cy="6336000"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1" name="Picture 1"/>
@@ -78,180 +147,6 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="3960000" cy="5760000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="3960000" cy="7200000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="3960000" cy="7200000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 4"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="3960000" cy="7200000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 5"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="3960000" cy="7200000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 6"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="7200000" cy="3600000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 7"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -608,14 +503,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>生産本部</t>
+          <t>営業本部</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>---</t>
+          <t>営業企画部</t>
         </is>
       </c>
     </row>
@@ -652,85 +547,121 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView showGridLines="1" showRowColHeaders="1" tabSelected="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="15" width="8.43"/>
+    <col min="16" max="16" bestFit="1" customWidth="1" hidden="false" width="30.711"/>
+  </cols>
   <sheetData>
     <row customHeight="1" ht="32" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>「高ストレス者割合」の部署間比較：</t>
+          <t>基本:総合健康リスク</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>部署</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>color_this</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>平均値</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>他5</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>他の部署</t>
-        </is>
-      </c>
-      <c r="C4">
-        <v>28.9</v>
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>総合健康リスク</t>
+        </is>
+      </c>
+      <c r="P3" s="2" t="inlineStr">
+        <is>
+          <t>総合健康リスク/total_risk_long/total_risk_cross/total_risk_old</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>他4</t>
+          <t>部署</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>他の部署</t>
-        </is>
-      </c>
-      <c r="C5">
-        <v>28.3</v>
+          <t>color_this</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>平均値</t>
+        </is>
+      </c>
+      <c r="P5" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Q5" s="9" t="inlineStr">
+        <is>
+          <t>全体</t>
+        </is>
+      </c>
+      <c r="R5" s="9" t="inlineStr">
+        <is>
+          <t>全体</t>
+        </is>
+      </c>
+      <c r="S5" s="9" t="inlineStr">
+        <is>
+          <t>営業本部-営業企画部</t>
+        </is>
+      </c>
+      <c r="T5" s="4" t="inlineStr">
+        <is>
+          <t>営業本部-営業企画部</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>管理本部</t>
+          <t>他20</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>対象</t>
+          <t>他の部署</t>
         </is>
       </c>
       <c r="C6">
-        <v>27.5</v>
+        <v>104</v>
+      </c>
+      <c r="P6" s="7" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="Q6" s="11" t="inlineStr">
+        <is>
+          <t>今回</t>
+        </is>
+      </c>
+      <c r="R6" s="11" t="inlineStr">
+        <is>
+          <t>今回</t>
+        </is>
+      </c>
+      <c r="S6" s="11" t="inlineStr">
+        <is>
+          <t>前回</t>
+        </is>
+      </c>
+      <c r="T6" s="8" t="inlineStr">
+        <is>
+          <t>前回</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>他3</t>
+          <t>他18</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -739,28 +670,62 @@
         </is>
       </c>
       <c r="C7">
-        <v>27.4</v>
+        <v>103</v>
+      </c>
+      <c r="P7" s="7" t="inlineStr">
+        <is>
+          <t>総合健康リスク(縦断)</t>
+        </is>
+      </c>
+      <c r="Q7" s="11">
+        <v>99</v>
+      </c>
+      <c r="R7" s="11">
+        <v>99</v>
+      </c>
+      <c r="S7" s="11">
+        <v>98</v>
+      </c>
+      <c r="T7" s="8">
+        <v>101</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>事業場平均</t>
+          <t>他19</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>事業場平均</t>
+          <t>他の部署</t>
         </is>
       </c>
       <c r="C8">
-        <v>27.4</v>
+        <v>103</v>
+      </c>
+      <c r="P8" s="7" t="inlineStr">
+        <is>
+          <t>総合健康リスク(横断)</t>
+        </is>
+      </c>
+      <c r="Q8" s="11">
+        <v>96</v>
+      </c>
+      <c r="R8" s="11">
+        <v>94</v>
+      </c>
+      <c r="S8" s="11">
+        <v>93</v>
+      </c>
+      <c r="T8" s="8">
+        <v>97</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>他2</t>
+          <t>他16</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -769,25 +734,306 @@
         </is>
       </c>
       <c r="C9">
-        <v>27.1</v>
+        <v>102</v>
+      </c>
+      <c r="P9" s="7" t="inlineStr">
+        <is>
+          <t>総合健康リスク(旧)</t>
+        </is>
+      </c>
+      <c r="Q9" s="11">
+        <v>101</v>
+      </c>
+      <c r="R9" s="11">
+        <v>101</v>
+      </c>
+      <c r="S9" s="11">
+        <v>99</v>
+      </c>
+      <c r="T9" s="8">
+        <v>102</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>他17</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>他の部署</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>102</v>
+      </c>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="6"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>他12</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>他の部署</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>他13</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>他の部署</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>他14</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>他の部署</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>他15</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>他の部署</t>
+        </is>
+      </c>
+      <c r="C14">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>他10</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>他の部署</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>他11</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>他の部署</t>
+        </is>
+      </c>
+      <c r="C16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>他9</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>他の部署</t>
+        </is>
+      </c>
+      <c r="C17">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>事業場平均</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>事業場平均</t>
+        </is>
+      </c>
+      <c r="C18">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>他5</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>他の部署</t>
+        </is>
+      </c>
+      <c r="C19">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>他6</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>他の部署</t>
+        </is>
+      </c>
+      <c r="C20">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>他7</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>他の部署</t>
+        </is>
+      </c>
+      <c r="C21">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>他8</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>他の部署</t>
+        </is>
+      </c>
+      <c r="C22">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>営業本部-営業企画部</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>対象</t>
+        </is>
+      </c>
+      <c r="C23">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>他3</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>他の部署</t>
+        </is>
+      </c>
+      <c r="C24">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>他4</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>他の部署</t>
+        </is>
+      </c>
+      <c r="C25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>他1</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>他の部署</t>
-        </is>
-      </c>
-      <c r="C10">
-        <v>25.3</v>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>他の部署</t>
+        </is>
+      </c>
+      <c r="C26">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>他2</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>他の部署</t>
+        </is>
+      </c>
+      <c r="C27">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+  </mergeCells>
   <printOptions gridLines="1" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>